<commit_message>
GUI improved page setup
</commit_message>
<xml_diff>
--- a/documentation/VariableClass.xlsx
+++ b/documentation/VariableClass.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/x/Documents/003_Tools/006_ControlledLandingSim/BlueBook-Descent-and-Landing-Analysis-Toolkit-DaLAT/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCA7790-9F7B-9B44-B6F4-3A1B0EBD1C8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4126A1E-347B-434A-9341-7D1085AFE60E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18800" yWindow="460" windowWidth="10000" windowHeight="16220" xr2:uid="{E3BD1D45-5A6E-B048-B8D3-3F4E8AF28D79}"/>
   </bookViews>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE70A57-7E49-BC47-BA76-739B6BB2838F}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
New links added, new aero functions, bug fixes
</commit_message>
<xml_diff>
--- a/documentation/VariableClass.xlsx
+++ b/documentation/VariableClass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/x/Documents/003_Tools/006_ControlledLandingSim/BlueBook-Descent-and-Landing-Analysis-Toolkit-DaLAT/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4126A1E-347B-434A-9341-7D1085AFE60E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5417B0-085E-A840-B527-3AAA7233C536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="460" windowWidth="10000" windowHeight="16220" xr2:uid="{E3BD1D45-5A6E-B048-B8D3-3F4E8AF28D79}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{E3BD1D45-5A6E-B048-B8D3-3F4E8AF28D79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -470,13 +470,6 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -650,11 +643,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE70A57-7E49-BC47-BA76-739B6BB2838F}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1506,7 +1499,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="19" t="s">
         <v>64</v>
       </c>
       <c r="C56" s="8" t="s">
@@ -1768,32 +1761,32 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="18"/>
-      <c r="B85" s="18" t="s">
+      <c r="A85" s="17"/>
+      <c r="B85" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D85" s="18" t="s">
+      <c r="D85" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="E85" s="18" t="s">
+      <c r="E85" s="17" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="18"/>
-      <c r="B86" s="18" t="s">
+      <c r="A86" s="17"/>
+      <c r="B86" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="C86" s="19" t="s">
+      <c r="C86" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D86" s="18" t="s">
+      <c r="D86" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E86" s="18" t="s">
+      <c r="E86" s="17" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>